<commit_message>
Fully incorporated LabelEncoding & Updated Slides and Report with results
</commit_message>
<xml_diff>
--- a/Training Results.xlsx
+++ b/Training Results.xlsx
@@ -11,14 +11,17 @@
     <sheet name="No PCA &amp; Sampling - Dum" sheetId="2" r:id="rId2"/>
     <sheet name="PCA &amp; No Sampling - Dum" sheetId="3" r:id="rId3"/>
     <sheet name="PCA &amp; Sampling - Dum" sheetId="4" r:id="rId4"/>
-    <sheet name="No PCA &amp; Sampling - No Dum" sheetId="5" r:id="rId5"/>
+    <sheet name="No PCA or Sampling - No Dum" sheetId="5" r:id="rId5"/>
+    <sheet name="No PCA &amp; Sampling - No Dum" sheetId="6" r:id="rId6"/>
+    <sheet name="PCA &amp; No Sampling - No Dum" sheetId="7" r:id="rId7"/>
+    <sheet name="PCA &amp; Sampling - No Dum" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="3">
   <si>
     <t>Logistic Regresion</t>
   </si>
@@ -406,13 +409,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.7105032132849554</v>
+        <v>0.7328008386888083</v>
       </c>
       <c r="C2">
-        <v>0.7236869180914373</v>
+        <v>0.7182267694502146</v>
       </c>
       <c r="D2">
-        <v>0.6856534523814164</v>
+        <v>0.6666712784158447</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -420,13 +423,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.7442146962254014</v>
+        <v>0.754846626109054</v>
       </c>
       <c r="C3">
-        <v>0.7288580561532493</v>
+        <v>0.7296295728980202</v>
       </c>
       <c r="D3">
-        <v>0.6910829763334932</v>
+        <v>0.6998728061898157</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -434,13 +437,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.7419805709387143</v>
+        <v>0.7492060273464546</v>
       </c>
       <c r="C4">
-        <v>0.719921326300447</v>
+        <v>0.7130707888411264</v>
       </c>
       <c r="D4">
-        <v>0.6853436843025295</v>
+        <v>0.6789985597219869</v>
       </c>
     </row>
   </sheetData>
@@ -472,13 +475,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.8981188350331852</v>
+        <v>0.8991316141252031</v>
       </c>
       <c r="C2">
-        <v>0.5672494163863893</v>
+        <v>0.6062146957609581</v>
       </c>
       <c r="D2">
-        <v>0.6815103998191675</v>
+        <v>0.6681878164082138</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -486,13 +489,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.9016121871632901</v>
+        <v>0.8977984332326566</v>
       </c>
       <c r="C3">
-        <v>0.71075073234881</v>
+        <v>0.7087584538846892</v>
       </c>
       <c r="D3">
-        <v>0.7507112455761252</v>
+        <v>0.752196484509269</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -500,13 +503,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.9064641919219492</v>
+        <v>0.9081247104456669</v>
       </c>
       <c r="C4">
-        <v>0.6884433976570333</v>
+        <v>0.710620984889252</v>
       </c>
       <c r="D4">
-        <v>0.7475676845193235</v>
+        <v>0.7410838929053289</v>
       </c>
     </row>
   </sheetData>
@@ -541,10 +544,10 @@
         <v>0.5</v>
       </c>
       <c r="C2">
-        <v>0.5309032078288015</v>
+        <v>0.5241990365991013</v>
       </c>
       <c r="D2">
-        <v>0.5007049545775184</v>
+        <v>0.5057262920367432</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -555,10 +558,10 @@
         <v>0.5</v>
       </c>
       <c r="C3">
-        <v>0.5371017326545779</v>
+        <v>0.5439637384008177</v>
       </c>
       <c r="D3">
-        <v>0.5063251011852192</v>
+        <v>0.5041115301326291</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -569,10 +572,10 @@
         <v>0.5</v>
       </c>
       <c r="C4">
-        <v>0.5322113612513931</v>
+        <v>0.5295187669020757</v>
       </c>
       <c r="D4">
-        <v>0.5049332259446669</v>
+        <v>0.5061023341830998</v>
       </c>
     </row>
   </sheetData>
@@ -604,13 +607,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.5727590211659801</v>
+        <v>0.5703971105767545</v>
       </c>
       <c r="C2">
-        <v>0.5182890865229101</v>
+        <v>0.5171297512383519</v>
       </c>
       <c r="D2">
-        <v>0.503923208530307</v>
+        <v>0.5082944452455465</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -618,13 +621,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5704723761167336</v>
+        <v>0.5761295204104899</v>
       </c>
       <c r="C3">
-        <v>0.5178692568506633</v>
+        <v>0.5305166704308398</v>
       </c>
       <c r="D3">
-        <v>0.5086011910881585</v>
+        <v>0.5101064094142234</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -632,13 +635,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.5734740501416526</v>
+        <v>0.5734577039354652</v>
       </c>
       <c r="C4">
-        <v>0.5188177525628684</v>
+        <v>0.5172688215141598</v>
       </c>
       <c r="D4">
-        <v>0.5068834465081629</v>
+        <v>0.5051671342469406</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +651,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -670,13 +673,239 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.7360908410661325</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.7358185594974103</v>
       </c>
       <c r="D2">
-        <v>0.9996570644718793</v>
+        <v>0.7801402036704326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.7623299701632741</v>
+      </c>
+      <c r="C3">
+        <v>0.8183232386063142</v>
+      </c>
+      <c r="D3">
+        <v>0.7953141788673466</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.7421561252543215</v>
+      </c>
+      <c r="C4">
+        <v>0.8075634211136422</v>
+      </c>
+      <c r="D4">
+        <v>0.7883506417993209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.8766352093409355</v>
+      </c>
+      <c r="C2">
+        <v>0.7706789599011655</v>
+      </c>
+      <c r="D2">
+        <v>0.7904237872723517</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.8800602079005679</v>
+      </c>
+      <c r="C3">
+        <v>0.7868627291667586</v>
+      </c>
+      <c r="D3">
+        <v>0.8126572908925519</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.8961957415257527</v>
+      </c>
+      <c r="C4">
+        <v>0.7900933246269107</v>
+      </c>
+      <c r="D4">
+        <v>0.8209197092470765</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>0.5202473001781045</v>
+      </c>
+      <c r="D2">
+        <v>0.5061405310396702</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.5258897135845804</v>
+      </c>
+      <c r="D3">
+        <v>0.5058532961461333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.5</v>
+      </c>
+      <c r="C4">
+        <v>0.5455169761456464</v>
+      </c>
+      <c r="D4">
+        <v>0.5076209164321281</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.5447909903309157</v>
+      </c>
+      <c r="C2">
+        <v>0.5169213066709276</v>
+      </c>
+      <c r="D2">
+        <v>0.5041336212104087</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.5561560588716121</v>
+      </c>
+      <c r="C3">
+        <v>0.519904074772212</v>
+      </c>
+      <c r="D3">
+        <v>0.5082789193179668</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.5541294770781681</v>
+      </c>
+      <c r="C4">
+        <v>0.5223841402569087</v>
+      </c>
+      <c r="D4">
+        <v>0.509912437903126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>